<commit_message>
added option for shade
</commit_message>
<xml_diff>
--- a/shifts_arranger.xlsx
+++ b/shifts_arranger.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eyal\Desktop\smart-shifts-system\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD6D7C2A-F983-4791-A2DA-D9668EAE0F7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{940FF450-84D8-4104-B58F-3E7F4FABC9EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="47">
   <si>
     <t>אייל</t>
   </si>
@@ -82,100 +82,124 @@
     <t>אליה</t>
   </si>
   <si>
-    <t>אגם</t>
-  </si>
-  <si>
     <t>רועי</t>
   </si>
   <si>
-    <t>14.7 Day Shift</t>
-  </si>
-  <si>
-    <t>14.7 Night Shift</t>
-  </si>
-  <si>
-    <t>15.7 Day Shift</t>
-  </si>
-  <si>
-    <t>15.7 Night Shift</t>
-  </si>
-  <si>
-    <t>16.7 Day Shift</t>
-  </si>
-  <si>
-    <t>16.7 Night Shift</t>
-  </si>
-  <si>
-    <t>17.7 Day Shift</t>
-  </si>
-  <si>
-    <t>17.7 Night Shift</t>
-  </si>
-  <si>
-    <t>18.7 Day Shift</t>
-  </si>
-  <si>
-    <t>18.7 Night Shift</t>
-  </si>
-  <si>
-    <t>19.7 Day Shift</t>
-  </si>
-  <si>
-    <t>19.7 Night Shift</t>
-  </si>
-  <si>
-    <t>20.7 Day Shift</t>
-  </si>
-  <si>
-    <t>20.7 Night Shift</t>
-  </si>
-  <si>
     <t>יום</t>
   </si>
   <si>
     <t>לילה</t>
   </si>
   <si>
-    <t>21.7 Day Shift</t>
-  </si>
-  <si>
-    <t>21.7 Night Shift</t>
-  </si>
-  <si>
-    <t>22.7 Day Shift</t>
-  </si>
-  <si>
-    <t>22.7 Night Shift</t>
-  </si>
-  <si>
-    <t>23.7 Day Shift</t>
-  </si>
-  <si>
-    <t>23.7 Night Shift</t>
-  </si>
-  <si>
-    <t>24.7 Day Shift</t>
-  </si>
-  <si>
-    <t>24.7 Night Shift</t>
-  </si>
-  <si>
-    <t>25.7 Day Shift</t>
-  </si>
-  <si>
-    <t>25.7 Night Shift</t>
-  </si>
-  <si>
-    <t>26.7 Day Shift</t>
-  </si>
-  <si>
-    <t>26.7 Night Shift</t>
-  </si>
-  <si>
-    <t>27.7 Day Shift</t>
-  </si>
-  <si>
-    <t>27.7 Night Shift</t>
+    <t>ירין</t>
+  </si>
+  <si>
+    <t>מילואים</t>
+  </si>
+  <si>
+    <t>יום ראשון</t>
+  </si>
+  <si>
+    <t>יום שני</t>
+  </si>
+  <si>
+    <t>יום שלישי</t>
+  </si>
+  <si>
+    <t>יום רביעי</t>
+  </si>
+  <si>
+    <t>יום חמישי</t>
+  </si>
+  <si>
+    <t>יום שישי</t>
+  </si>
+  <si>
+    <t>יום שבת</t>
+  </si>
+  <si>
+    <t>3.11 Day Shift</t>
+  </si>
+  <si>
+    <t>3.11 Night Shift</t>
+  </si>
+  <si>
+    <t>4.11 Day Shift</t>
+  </si>
+  <si>
+    <t>4.11 Night Shift</t>
+  </si>
+  <si>
+    <t>5.11 Day Shift</t>
+  </si>
+  <si>
+    <t>5.11 Night Shift</t>
+  </si>
+  <si>
+    <t>6.11 Day Shift</t>
+  </si>
+  <si>
+    <t>6.11 Night Shift</t>
+  </si>
+  <si>
+    <t>7.11 Day Shift</t>
+  </si>
+  <si>
+    <t>7.11 Night Shift</t>
+  </si>
+  <si>
+    <t>8.11 Day Shift</t>
+  </si>
+  <si>
+    <t>8.11 Night Shift</t>
+  </si>
+  <si>
+    <t>9.11 Day Shift</t>
+  </si>
+  <si>
+    <t>9.11 Night Shift</t>
+  </si>
+  <si>
+    <t>10.11 Day Shift</t>
+  </si>
+  <si>
+    <t>10.11 Night Shift</t>
+  </si>
+  <si>
+    <t>11.11 Day Shift</t>
+  </si>
+  <si>
+    <t>11.11 Night Shift</t>
+  </si>
+  <si>
+    <t>12.11 Day Shift</t>
+  </si>
+  <si>
+    <t>12.11 Night Shift</t>
+  </si>
+  <si>
+    <t>13.11 Day Shift</t>
+  </si>
+  <si>
+    <t>13.11 Night Shift</t>
+  </si>
+  <si>
+    <t>14.11 Day Shift</t>
+  </si>
+  <si>
+    <t>14.11 Night Shift</t>
+  </si>
+  <si>
+    <t>15.11 Day Shift</t>
+  </si>
+  <si>
+    <t>15.11 Night Shift</t>
+  </si>
+  <si>
+    <t>16.11 Day Shift</t>
+  </si>
+  <si>
+    <t>16.11 Night Shift</t>
   </si>
 </sst>
 </file>
@@ -206,7 +230,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -215,24 +239,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FFC9EBFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.249977111117893"/>
+        <fgColor rgb="FFE1F8FF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
+        <fgColor rgb="FFFEE97E"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFE7E3"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -255,24 +285,69 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFE7E3"/>
+      <color rgb="FFFDF6E6"/>
+      <color rgb="FFB6E3BC"/>
+      <color rgb="FFC9EBFF"/>
+      <color rgb="FF92D0CD"/>
+      <color rgb="FFFEE97E"/>
+      <color rgb="FFE1F8FF"/>
+      <color rgb="FFABB5FF"/>
+      <color rgb="FF7475B6"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -547,141 +622,158 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H87"/>
+  <dimension ref="A1:H88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="8" max="8" width="12.77734375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="4"/>
-      <c r="B1" s="4" t="str">
-        <f>A60</f>
-        <v>14.7</v>
-      </c>
-      <c r="C1" s="4" t="str">
-        <f>A62</f>
-        <v>15.7</v>
-      </c>
-      <c r="D1" s="4" t="str">
-        <f>A64</f>
-        <v>16.7</v>
-      </c>
-      <c r="E1" s="4" t="str">
-        <f>A66</f>
-        <v>17.7</v>
-      </c>
-      <c r="F1" s="4" t="str">
-        <f>A68</f>
-        <v>18.7</v>
-      </c>
-      <c r="G1" s="4" t="str">
-        <f>A70</f>
-        <v>19.7</v>
-      </c>
-      <c r="H1" s="4" t="str">
-        <f>A72</f>
-        <v>20.7</v>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="5"/>
+      <c r="B1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
+      <c r="A2" s="8"/>
+      <c r="B2" s="8" t="str">
+        <f>A61</f>
+        <v>3.11</v>
+      </c>
+      <c r="C2" s="8" t="str">
+        <f>A63</f>
+        <v>4.11</v>
+      </c>
+      <c r="D2" s="8" t="str">
+        <f>A65</f>
+        <v>5.11</v>
+      </c>
+      <c r="E2" s="8" t="str">
+        <f>A67</f>
+        <v>6.11</v>
+      </c>
+      <c r="F2" s="8" t="str">
+        <f>A69</f>
+        <v>7.11</v>
+      </c>
+      <c r="G2" s="8" t="str">
+        <f>A71</f>
+        <v>8.11</v>
+      </c>
+      <c r="H2" s="8" t="str">
+        <f>A73</f>
+        <v>9.11</v>
+      </c>
     </row>
     <row r="3" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
+      <c r="A3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
     </row>
     <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4" t="str">
-        <f>A74</f>
-        <v>21.7</v>
-      </c>
-      <c r="C4" s="4" t="str">
-        <f>A76</f>
-        <v>22.7</v>
-      </c>
-      <c r="D4" s="4" t="str">
-        <f>A78</f>
-        <v>23.7</v>
-      </c>
-      <c r="E4" s="4" t="str">
-        <f>A80</f>
-        <v>24.7</v>
-      </c>
-      <c r="F4" s="4" t="str">
-        <f>A82</f>
-        <v>25.7</v>
-      </c>
-      <c r="G4" s="4" t="str">
-        <f>A84</f>
-        <v>26.7</v>
-      </c>
-      <c r="H4" s="4" t="str">
-        <f>A86</f>
-        <v>27.7</v>
-      </c>
+      <c r="A4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
     </row>
     <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="7" t="str">
+        <f>A75</f>
+        <v>10.11</v>
+      </c>
+      <c r="C5" s="7" t="str">
+        <f>A77</f>
+        <v>11.11</v>
+      </c>
+      <c r="D5" s="7" t="str">
+        <f>A79</f>
+        <v>12.11</v>
+      </c>
+      <c r="E5" s="7" t="str">
+        <f>A81</f>
+        <v>13.11</v>
+      </c>
+      <c r="F5" s="7" t="str">
+        <f>A83</f>
+        <v>14.11</v>
+      </c>
+      <c r="G5" s="7" t="str">
+        <f>A85</f>
+        <v>15.11</v>
+      </c>
+      <c r="H5" s="7" t="str">
+        <f>A87</f>
+        <v>16.11</v>
+      </c>
     </row>
     <row r="6" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A60" t="str" cm="1">
-        <f t="array" ref="A60:C60">_xlfn.TEXTSPLIT('טבלת זמינות'!A2, " ")</f>
-        <v>14.7</v>
-      </c>
-      <c r="B60" t="str">
-        <v>Day</v>
-      </c>
-      <c r="C60" t="str">
-        <v>Shift</v>
-      </c>
+      <c r="A6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+    </row>
+    <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="str" cm="1">
-        <f t="array" ref="A61:C61">_xlfn.TEXTSPLIT('טבלת זמינות'!A3, " ")</f>
-        <v>14.7</v>
+        <f t="array" ref="A61:C61">_xlfn.TEXTSPLIT('טבלת זמינות'!A2, " ")</f>
+        <v>3.11</v>
       </c>
       <c r="B61" t="str">
-        <v>Night</v>
+        <v>Day</v>
       </c>
       <c r="C61" t="str">
         <v>Shift</v>
@@ -689,11 +781,11 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="str" cm="1">
-        <f t="array" ref="A62:C62">_xlfn.TEXTSPLIT('טבלת זמינות'!A4, " ")</f>
-        <v>15.7</v>
+        <f t="array" ref="A62:C62">_xlfn.TEXTSPLIT('טבלת זמינות'!A3, " ")</f>
+        <v>3.11</v>
       </c>
       <c r="B62" t="str">
-        <v>Day</v>
+        <v>Night</v>
       </c>
       <c r="C62" t="str">
         <v>Shift</v>
@@ -701,11 +793,11 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="str" cm="1">
-        <f t="array" ref="A63:C63">_xlfn.TEXTSPLIT('טבלת זמינות'!A5, " ")</f>
-        <v>15.7</v>
+        <f t="array" ref="A63:C63">_xlfn.TEXTSPLIT('טבלת זמינות'!A4, " ")</f>
+        <v>4.11</v>
       </c>
       <c r="B63" t="str">
-        <v>Night</v>
+        <v>Day</v>
       </c>
       <c r="C63" t="str">
         <v>Shift</v>
@@ -713,11 +805,11 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="str" cm="1">
-        <f t="array" ref="A64:C64">_xlfn.TEXTSPLIT('טבלת זמינות'!A6, " ")</f>
-        <v>16.7</v>
+        <f t="array" ref="A64:C64">_xlfn.TEXTSPLIT('טבלת זמינות'!A5, " ")</f>
+        <v>4.11</v>
       </c>
       <c r="B64" t="str">
-        <v>Day</v>
+        <v>Night</v>
       </c>
       <c r="C64" t="str">
         <v>Shift</v>
@@ -725,11 +817,11 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="str" cm="1">
-        <f t="array" ref="A65:C65">_xlfn.TEXTSPLIT('טבלת זמינות'!A7, " ")</f>
-        <v>16.7</v>
+        <f t="array" ref="A65:C65">_xlfn.TEXTSPLIT('טבלת זמינות'!A6, " ")</f>
+        <v>5.11</v>
       </c>
       <c r="B65" t="str">
-        <v>Night</v>
+        <v>Day</v>
       </c>
       <c r="C65" t="str">
         <v>Shift</v>
@@ -737,11 +829,11 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="str" cm="1">
-        <f t="array" ref="A66:C66">_xlfn.TEXTSPLIT('טבלת זמינות'!A8, " ")</f>
-        <v>17.7</v>
+        <f t="array" ref="A66:C66">_xlfn.TEXTSPLIT('טבלת זמינות'!A7, " ")</f>
+        <v>5.11</v>
       </c>
       <c r="B66" t="str">
-        <v>Day</v>
+        <v>Night</v>
       </c>
       <c r="C66" t="str">
         <v>Shift</v>
@@ -749,11 +841,11 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="str" cm="1">
-        <f t="array" ref="A67:C67">_xlfn.TEXTSPLIT('טבלת זמינות'!A9, " ")</f>
-        <v>17.7</v>
+        <f t="array" ref="A67:C67">_xlfn.TEXTSPLIT('טבלת זמינות'!A8, " ")</f>
+        <v>6.11</v>
       </c>
       <c r="B67" t="str">
-        <v>Night</v>
+        <v>Day</v>
       </c>
       <c r="C67" t="str">
         <v>Shift</v>
@@ -761,11 +853,11 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="str" cm="1">
-        <f t="array" ref="A68:C68">_xlfn.TEXTSPLIT('טבלת זמינות'!A10, " ")</f>
-        <v>18.7</v>
+        <f t="array" ref="A68:C68">_xlfn.TEXTSPLIT('טבלת זמינות'!A9, " ")</f>
+        <v>6.11</v>
       </c>
       <c r="B68" t="str">
-        <v>Day</v>
+        <v>Night</v>
       </c>
       <c r="C68" t="str">
         <v>Shift</v>
@@ -773,11 +865,11 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="str" cm="1">
-        <f t="array" ref="A69:C69">_xlfn.TEXTSPLIT('טבלת זמינות'!A11, " ")</f>
-        <v>18.7</v>
+        <f t="array" ref="A69:C69">_xlfn.TEXTSPLIT('טבלת זמינות'!A10, " ")</f>
+        <v>7.11</v>
       </c>
       <c r="B69" t="str">
-        <v>Night</v>
+        <v>Day</v>
       </c>
       <c r="C69" t="str">
         <v>Shift</v>
@@ -785,11 +877,11 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="str" cm="1">
-        <f t="array" ref="A70:C70">_xlfn.TEXTSPLIT('טבלת זמינות'!A12, " ")</f>
-        <v>19.7</v>
+        <f t="array" ref="A70:C70">_xlfn.TEXTSPLIT('טבלת זמינות'!A11, " ")</f>
+        <v>7.11</v>
       </c>
       <c r="B70" t="str">
-        <v>Day</v>
+        <v>Night</v>
       </c>
       <c r="C70" t="str">
         <v>Shift</v>
@@ -797,11 +889,11 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="str" cm="1">
-        <f t="array" ref="A71:C71">_xlfn.TEXTSPLIT('טבלת זמינות'!A13, " ")</f>
-        <v>19.7</v>
+        <f t="array" ref="A71:C71">_xlfn.TEXTSPLIT('טבלת זמינות'!A12, " ")</f>
+        <v>8.11</v>
       </c>
       <c r="B71" t="str">
-        <v>Night</v>
+        <v>Day</v>
       </c>
       <c r="C71" t="str">
         <v>Shift</v>
@@ -809,11 +901,11 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="str" cm="1">
-        <f t="array" ref="A72:C72">_xlfn.TEXTSPLIT('טבלת זמינות'!A14, " ")</f>
-        <v>20.7</v>
+        <f t="array" ref="A72:C72">_xlfn.TEXTSPLIT('טבלת זמינות'!A13, " ")</f>
+        <v>8.11</v>
       </c>
       <c r="B72" t="str">
-        <v>Day</v>
+        <v>Night</v>
       </c>
       <c r="C72" t="str">
         <v>Shift</v>
@@ -821,11 +913,11 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="str" cm="1">
-        <f t="array" ref="A73:C73">_xlfn.TEXTSPLIT('טבלת זמינות'!A15, " ")</f>
-        <v>20.7</v>
+        <f t="array" ref="A73:C73">_xlfn.TEXTSPLIT('טבלת זמינות'!A14, " ")</f>
+        <v>9.11</v>
       </c>
       <c r="B73" t="str">
-        <v>Night</v>
+        <v>Day</v>
       </c>
       <c r="C73" t="str">
         <v>Shift</v>
@@ -833,11 +925,11 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="str" cm="1">
-        <f t="array" ref="A74:C74">_xlfn.TEXTSPLIT('טבלת זמינות'!A16, " ")</f>
-        <v>21.7</v>
+        <f t="array" ref="A74:C74">_xlfn.TEXTSPLIT('טבלת זמינות'!A15, " ")</f>
+        <v>9.11</v>
       </c>
       <c r="B74" t="str">
-        <v>Day</v>
+        <v>Night</v>
       </c>
       <c r="C74" t="str">
         <v>Shift</v>
@@ -845,11 +937,11 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="str" cm="1">
-        <f t="array" ref="A75:C75">_xlfn.TEXTSPLIT('טבלת זמינות'!A17, " ")</f>
-        <v>21.7</v>
+        <f t="array" ref="A75:C75">_xlfn.TEXTSPLIT('טבלת זמינות'!A16, " ")</f>
+        <v>10.11</v>
       </c>
       <c r="B75" t="str">
-        <v>Night</v>
+        <v>Day</v>
       </c>
       <c r="C75" t="str">
         <v>Shift</v>
@@ -857,11 +949,11 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="str" cm="1">
-        <f t="array" ref="A76:C76">_xlfn.TEXTSPLIT('טבלת זמינות'!A18, " ")</f>
-        <v>22.7</v>
+        <f t="array" ref="A76:C76">_xlfn.TEXTSPLIT('טבלת זמינות'!A17, " ")</f>
+        <v>10.11</v>
       </c>
       <c r="B76" t="str">
-        <v>Day</v>
+        <v>Night</v>
       </c>
       <c r="C76" t="str">
         <v>Shift</v>
@@ -869,11 +961,11 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="str" cm="1">
-        <f t="array" ref="A77:C77">_xlfn.TEXTSPLIT('טבלת זמינות'!A19, " ")</f>
-        <v>22.7</v>
+        <f t="array" ref="A77:C77">_xlfn.TEXTSPLIT('טבלת זמינות'!A18, " ")</f>
+        <v>11.11</v>
       </c>
       <c r="B77" t="str">
-        <v>Night</v>
+        <v>Day</v>
       </c>
       <c r="C77" t="str">
         <v>Shift</v>
@@ -881,11 +973,11 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="str" cm="1">
-        <f t="array" ref="A78:C78">_xlfn.TEXTSPLIT('טבלת זמינות'!A20, " ")</f>
-        <v>23.7</v>
+        <f t="array" ref="A78:C78">_xlfn.TEXTSPLIT('טבלת זמינות'!A19, " ")</f>
+        <v>11.11</v>
       </c>
       <c r="B78" t="str">
-        <v>Day</v>
+        <v>Night</v>
       </c>
       <c r="C78" t="str">
         <v>Shift</v>
@@ -893,11 +985,11 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" t="str" cm="1">
-        <f t="array" ref="A79:C79">_xlfn.TEXTSPLIT('טבלת זמינות'!A21, " ")</f>
-        <v>23.7</v>
+        <f t="array" ref="A79:C79">_xlfn.TEXTSPLIT('טבלת זמינות'!A20, " ")</f>
+        <v>12.11</v>
       </c>
       <c r="B79" t="str">
-        <v>Night</v>
+        <v>Day</v>
       </c>
       <c r="C79" t="str">
         <v>Shift</v>
@@ -905,11 +997,11 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" t="str" cm="1">
-        <f t="array" ref="A80:C80">_xlfn.TEXTSPLIT('טבלת זמינות'!A22, " ")</f>
-        <v>24.7</v>
+        <f t="array" ref="A80:C80">_xlfn.TEXTSPLIT('טבלת זמינות'!A21, " ")</f>
+        <v>12.11</v>
       </c>
       <c r="B80" t="str">
-        <v>Day</v>
+        <v>Night</v>
       </c>
       <c r="C80" t="str">
         <v>Shift</v>
@@ -917,11 +1009,11 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="str" cm="1">
-        <f t="array" ref="A81:C81">_xlfn.TEXTSPLIT('טבלת זמינות'!A23, " ")</f>
-        <v>24.7</v>
+        <f t="array" ref="A81:C81">_xlfn.TEXTSPLIT('טבלת זמינות'!A22, " ")</f>
+        <v>13.11</v>
       </c>
       <c r="B81" t="str">
-        <v>Night</v>
+        <v>Day</v>
       </c>
       <c r="C81" t="str">
         <v>Shift</v>
@@ -929,11 +1021,11 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" t="str" cm="1">
-        <f t="array" ref="A82:C82">_xlfn.TEXTSPLIT('טבלת זמינות'!A24, " ")</f>
-        <v>25.7</v>
+        <f t="array" ref="A82:C82">_xlfn.TEXTSPLIT('טבלת זמינות'!A23, " ")</f>
+        <v>13.11</v>
       </c>
       <c r="B82" t="str">
-        <v>Day</v>
+        <v>Night</v>
       </c>
       <c r="C82" t="str">
         <v>Shift</v>
@@ -941,11 +1033,11 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" t="str" cm="1">
-        <f t="array" ref="A83:C83">_xlfn.TEXTSPLIT('טבלת זמינות'!A25, " ")</f>
-        <v>25.7</v>
+        <f t="array" ref="A83:C83">_xlfn.TEXTSPLIT('טבלת זמינות'!A24, " ")</f>
+        <v>14.11</v>
       </c>
       <c r="B83" t="str">
-        <v>Night</v>
+        <v>Day</v>
       </c>
       <c r="C83" t="str">
         <v>Shift</v>
@@ -953,11 +1045,11 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" t="str" cm="1">
-        <f t="array" ref="A84:C84">_xlfn.TEXTSPLIT('טבלת זמינות'!A26, " ")</f>
-        <v>26.7</v>
+        <f t="array" ref="A84:C84">_xlfn.TEXTSPLIT('טבלת זמינות'!A25, " ")</f>
+        <v>14.11</v>
       </c>
       <c r="B84" t="str">
-        <v>Day</v>
+        <v>Night</v>
       </c>
       <c r="C84" t="str">
         <v>Shift</v>
@@ -965,11 +1057,11 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" t="str" cm="1">
-        <f t="array" ref="A85:C85">_xlfn.TEXTSPLIT('טבלת זמינות'!A27, " ")</f>
-        <v>26.7</v>
+        <f t="array" ref="A85:C85">_xlfn.TEXTSPLIT('טבלת זמינות'!A26, " ")</f>
+        <v>15.11</v>
       </c>
       <c r="B85" t="str">
-        <v>Night</v>
+        <v>Day</v>
       </c>
       <c r="C85" t="str">
         <v>Shift</v>
@@ -977,11 +1069,11 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" t="str" cm="1">
-        <f t="array" ref="A86:C86">_xlfn.TEXTSPLIT('טבלת זמינות'!A28, " ")</f>
-        <v>27.7</v>
+        <f t="array" ref="A86:C86">_xlfn.TEXTSPLIT('טבלת זמינות'!A27, " ")</f>
+        <v>15.11</v>
       </c>
       <c r="B86" t="str">
-        <v>Day</v>
+        <v>Night</v>
       </c>
       <c r="C86" t="str">
         <v>Shift</v>
@@ -989,18 +1081,31 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" t="str" cm="1">
-        <f t="array" ref="A87:C87">_xlfn.TEXTSPLIT('טבלת זמינות'!A29, " ")</f>
-        <v>27.7</v>
+        <f t="array" ref="A87:C87">_xlfn.TEXTSPLIT('טבלת זמינות'!A28, " ")</f>
+        <v>16.11</v>
       </c>
       <c r="B87" t="str">
+        <v>Day</v>
+      </c>
+      <c r="C87" t="str">
+        <v>Shift</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A88" t="str" cm="1">
+        <f t="array" ref="A88:C88">_xlfn.TEXTSPLIT('טבלת זמינות'!A29, " ")</f>
+        <v>16.11</v>
+      </c>
+      <c r="B88" t="str">
         <v>Night</v>
       </c>
-      <c r="C87" t="str">
+      <c r="C88" t="str">
         <v>Shift</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="28">
@@ -1008,169 +1113,169 @@
           <x14:formula1>
             <xm:f>'טבלת זמינות'!$B$2:$W$2</xm:f>
           </x14:formula1>
-          <xm:sqref>B2</xm:sqref>
+          <xm:sqref>B3</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00804ABC-9A1C-4B62-AF14-472D18B2696E}">
           <x14:formula1>
             <xm:f>'טבלת זמינות'!$B$4:$W$4</xm:f>
           </x14:formula1>
-          <xm:sqref>C2</xm:sqref>
+          <xm:sqref>C3</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B4C128FB-0C12-454A-A575-30D5106CBCEB}">
           <x14:formula1>
             <xm:f>'טבלת זמינות'!$B$3:$W$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B3</xm:sqref>
+          <xm:sqref>B4</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D2FB89FD-97DD-40F5-8FE1-7E12FBF02D21}">
           <x14:formula1>
             <xm:f>'טבלת זמינות'!$B$5:$W$5</xm:f>
           </x14:formula1>
-          <xm:sqref>C3</xm:sqref>
+          <xm:sqref>C4</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C6CE8307-3281-4019-8FE7-FA80220CC175}">
           <x14:formula1>
             <xm:f>'טבלת זמינות'!$B$7:$W$7</xm:f>
           </x14:formula1>
+          <xm:sqref>D4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F1038E5D-4A34-4A0B-9938-2DFFD3ECA426}">
+          <x14:formula1>
+            <xm:f>'טבלת זמינות'!$B$6:$W$6</xm:f>
+          </x14:formula1>
           <xm:sqref>D3</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F1038E5D-4A34-4A0B-9938-2DFFD3ECA426}">
-          <x14:formula1>
-            <xm:f>'טבלת זמינות'!$B$6:$W$6</xm:f>
-          </x14:formula1>
-          <xm:sqref>D2</xm:sqref>
-        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{39A47CAE-572B-4FCD-8DC5-44C6E407056A}">
           <x14:formula1>
             <xm:f>'טבלת זמינות'!$B$8:$W$8</xm:f>
           </x14:formula1>
-          <xm:sqref>E2</xm:sqref>
+          <xm:sqref>E3</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D7E786EE-2284-4BCF-99CC-45B1D2246923}">
           <x14:formula1>
             <xm:f>'טבלת זמינות'!$B$9:$W$9</xm:f>
           </x14:formula1>
-          <xm:sqref>E3</xm:sqref>
+          <xm:sqref>E4</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7AEE15A3-D32B-4F72-AE91-DC38EB146CFA}">
           <x14:formula1>
             <xm:f>'טבלת זמינות'!$B$10:$W$10</xm:f>
           </x14:formula1>
-          <xm:sqref>F2</xm:sqref>
+          <xm:sqref>F3</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5F85F2D2-C9E0-4C98-BEF9-AB01FED144E7}">
           <x14:formula1>
             <xm:f>'טבלת זמינות'!$B$11:$W$11</xm:f>
           </x14:formula1>
-          <xm:sqref>F3</xm:sqref>
+          <xm:sqref>F4</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{97C0A6B8-954E-4E35-AD65-A0BA79A23A35}">
           <x14:formula1>
             <xm:f>'טבלת זמינות'!$B$12:$W$12</xm:f>
           </x14:formula1>
-          <xm:sqref>G2</xm:sqref>
+          <xm:sqref>G3</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{01985C42-D387-4017-A60D-CA3360C5AB58}">
           <x14:formula1>
             <xm:f>'טבלת זמינות'!$B$13:$W$13</xm:f>
           </x14:formula1>
-          <xm:sqref>G3</xm:sqref>
+          <xm:sqref>G4</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{44CB5E03-2AB4-469B-A82C-76E529DD9E51}">
           <x14:formula1>
             <xm:f>'טבלת זמינות'!$B$14:$W$14</xm:f>
           </x14:formula1>
-          <xm:sqref>H2</xm:sqref>
+          <xm:sqref>H3</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7E1DCB0E-51BE-4B60-85FB-04F66348EB65}">
           <x14:formula1>
             <xm:f>'טבלת זמינות'!$B$15:$W$15</xm:f>
           </x14:formula1>
-          <xm:sqref>H3</xm:sqref>
+          <xm:sqref>H4</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C62FCBE8-E95B-43F6-8DDD-24788FE472A2}">
           <x14:formula1>
             <xm:f>'טבלת זמינות'!$B$16:$W$16</xm:f>
           </x14:formula1>
-          <xm:sqref>B5</xm:sqref>
+          <xm:sqref>B6</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B83063B7-94BA-49D7-90BB-8ADEF65480BF}">
           <x14:formula1>
             <xm:f>'טבלת זמינות'!$B$17:$W$17</xm:f>
           </x14:formula1>
-          <xm:sqref>B6</xm:sqref>
+          <xm:sqref>B7</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6A6A3BB7-5A39-4F61-8583-DE1153EE94AE}">
           <x14:formula1>
             <xm:f>'טבלת זמינות'!$B$18:$W$18</xm:f>
           </x14:formula1>
-          <xm:sqref>C5</xm:sqref>
+          <xm:sqref>C6</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4524B2BF-3147-42D7-98E1-DDF80CAF090F}">
           <x14:formula1>
             <xm:f>'טבלת זמינות'!$B$19:$W$19</xm:f>
           </x14:formula1>
-          <xm:sqref>C6</xm:sqref>
+          <xm:sqref>C7</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FEF7B231-BC48-4D2C-AEF2-80A4F8C7D55B}">
           <x14:formula1>
             <xm:f>'טבלת זמינות'!$B$20:$W$20</xm:f>
           </x14:formula1>
-          <xm:sqref>D5</xm:sqref>
+          <xm:sqref>D6</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9A9A2D4F-E79A-4135-9B86-E90FD4A7F3C3}">
           <x14:formula1>
             <xm:f>'טבלת זמינות'!$B$21:$W$21</xm:f>
           </x14:formula1>
-          <xm:sqref>D6</xm:sqref>
+          <xm:sqref>D7</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{45080AA0-CEA8-4EEF-8DA9-96FDA4DD4831}">
           <x14:formula1>
             <xm:f>'טבלת זמינות'!$B$22:$W$22</xm:f>
           </x14:formula1>
-          <xm:sqref>E5</xm:sqref>
+          <xm:sqref>E6</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{383FAFD2-9A0E-4A05-B4E8-CC0380AC3CE9}">
           <x14:formula1>
             <xm:f>'טבלת זמינות'!$B$23:$W$23</xm:f>
           </x14:formula1>
-          <xm:sqref>E6</xm:sqref>
+          <xm:sqref>E7</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1D003611-EFB2-40FE-B83C-6AF6AF0ECE34}">
           <x14:formula1>
             <xm:f>'טבלת זמינות'!$B$24:$W$24</xm:f>
           </x14:formula1>
-          <xm:sqref>F5</xm:sqref>
+          <xm:sqref>F6</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{15B2B50E-BF28-4C9E-A19F-8EDA9B4794E6}">
           <x14:formula1>
             <xm:f>'טבלת זמינות'!$B$25:$W$25</xm:f>
           </x14:formula1>
-          <xm:sqref>F6</xm:sqref>
+          <xm:sqref>F7</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{70F3AA3A-F0B9-44B8-8D7B-A5B02DC0F08D}">
           <x14:formula1>
             <xm:f>'טבלת זמינות'!$B$26:$W$26</xm:f>
           </x14:formula1>
-          <xm:sqref>G5</xm:sqref>
+          <xm:sqref>G6</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{601EC61D-10B9-4285-848A-41B3010F9044}">
           <x14:formula1>
             <xm:f>'טבלת זמינות'!$B$27:$W$27</xm:f>
           </x14:formula1>
-          <xm:sqref>G6</xm:sqref>
+          <xm:sqref>G7</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0433CB6D-6341-4012-A335-8E20E8A9C649}">
           <x14:formula1>
             <xm:f>'טבלת זמינות'!$B$28:$W$28</xm:f>
           </x14:formula1>
-          <xm:sqref>H5</xm:sqref>
+          <xm:sqref>H6</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{930AA88C-8076-47F5-972F-F17D602F2047}">
           <x14:formula1>
             <xm:f>'טבלת זמינות'!$B$29:$W$29</xm:f>
           </x14:formula1>
-          <xm:sqref>H6</xm:sqref>
+          <xm:sqref>H7</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1180,23 +1285,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{703A9C9D-E287-4DB6-89F4-25B27FC47FFF}">
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.44140625" customWidth="1"/>
+    <col min="11" max="11" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -1211,191 +1317,206 @@
         <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="F5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" t="s">
+        <v>5</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" t="s">
+        <v>5</v>
+      </c>
+      <c r="H6" t="s">
+        <v>0</v>
+      </c>
+      <c r="I6" t="s">
+        <v>1</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="D7" t="s">
         <v>2</v>
       </c>
-      <c r="E3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I3" t="s">
-        <v>7</v>
-      </c>
-      <c r="J3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H4" t="s">
-        <v>6</v>
-      </c>
-      <c r="I4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F5" t="s">
-        <v>4</v>
-      </c>
-      <c r="H5" t="s">
-        <v>6</v>
-      </c>
-      <c r="I5" t="s">
-        <v>7</v>
-      </c>
-      <c r="J5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="E7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" t="s">
+        <v>4</v>
+      </c>
+      <c r="H7" t="s">
         <v>0</v>
       </c>
-      <c r="C6" t="s">
-        <v>1</v>
-      </c>
-      <c r="E6" t="s">
-        <v>3</v>
-      </c>
-      <c r="F6" t="s">
-        <v>4</v>
-      </c>
-      <c r="H6" t="s">
-        <v>6</v>
-      </c>
-      <c r="I6" t="s">
-        <v>7</v>
-      </c>
-      <c r="J6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" t="s">
-        <v>1</v>
-      </c>
-      <c r="F7" t="s">
-        <v>4</v>
-      </c>
-      <c r="H7" t="s">
-        <v>6</v>
-      </c>
       <c r="I7" t="s">
-        <v>7</v>
-      </c>
-      <c r="J7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D8" t="s">
         <v>2</v>
       </c>
+      <c r="E8" t="s">
+        <v>3</v>
+      </c>
       <c r="F8" t="s">
         <v>4</v>
       </c>
-      <c r="H8" t="s">
-        <v>6</v>
-      </c>
       <c r="I8" t="s">
-        <v>7</v>
-      </c>
-      <c r="J8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="B9" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D9" t="s">
         <v>2</v>
@@ -1403,28 +1524,22 @@
       <c r="E9" t="s">
         <v>3</v>
       </c>
-      <c r="F9" t="s">
-        <v>4</v>
-      </c>
-      <c r="H9" t="s">
-        <v>6</v>
-      </c>
       <c r="I9" t="s">
-        <v>7</v>
-      </c>
-      <c r="J9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D10" t="s">
         <v>2</v>
@@ -1432,77 +1547,77 @@
       <c r="E10" t="s">
         <v>3</v>
       </c>
-      <c r="F10" t="s">
-        <v>4</v>
-      </c>
       <c r="H10" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I10" t="s">
-        <v>7</v>
-      </c>
-      <c r="J10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="B11" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D11" t="s">
         <v>2</v>
       </c>
-      <c r="F11" t="s">
-        <v>4</v>
+      <c r="E11" t="s">
+        <v>3</v>
       </c>
       <c r="H11" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I11" t="s">
-        <v>7</v>
-      </c>
-      <c r="J11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="B12" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D12" t="s">
         <v>2</v>
       </c>
+      <c r="E12" t="s">
+        <v>3</v>
+      </c>
       <c r="F12" t="s">
         <v>4</v>
       </c>
+      <c r="G12" t="s">
+        <v>5</v>
+      </c>
       <c r="H12" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I12" t="s">
-        <v>7</v>
-      </c>
-      <c r="J12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="B13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C13" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D13" t="s">
         <v>2</v>
@@ -1513,25 +1628,25 @@
       <c r="F13" t="s">
         <v>4</v>
       </c>
+      <c r="G13" t="s">
+        <v>5</v>
+      </c>
       <c r="H13" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I13" t="s">
-        <v>7</v>
-      </c>
-      <c r="J13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="B14" t="s">
-        <v>0</v>
-      </c>
-      <c r="C14" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D14" t="s">
         <v>2</v>
@@ -1542,51 +1657,54 @@
       <c r="F14" t="s">
         <v>4</v>
       </c>
+      <c r="G14" t="s">
+        <v>5</v>
+      </c>
       <c r="H14" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I14" t="s">
-        <v>7</v>
-      </c>
-      <c r="J14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" t="s">
+        <v>3</v>
+      </c>
+      <c r="F15" t="s">
+        <v>4</v>
+      </c>
+      <c r="G15" t="s">
+        <v>5</v>
+      </c>
+      <c r="H15" t="s">
         <v>0</v>
       </c>
-      <c r="D15" t="s">
-        <v>2</v>
-      </c>
-      <c r="E15" t="s">
-        <v>3</v>
-      </c>
-      <c r="F15" t="s">
-        <v>4</v>
-      </c>
-      <c r="H15" t="s">
-        <v>6</v>
-      </c>
       <c r="I15" t="s">
-        <v>7</v>
-      </c>
-      <c r="J15" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>25</v>
+        <v>33</v>
+      </c>
+      <c r="B16" t="s">
+        <v>6</v>
       </c>
       <c r="C16" t="s">
-        <v>1</v>
-      </c>
-      <c r="D16" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E16" t="s">
         <v>3</v>
@@ -1594,28 +1712,22 @@
       <c r="F16" t="s">
         <v>4</v>
       </c>
-      <c r="H16" t="s">
-        <v>6</v>
-      </c>
       <c r="I16" t="s">
-        <v>7</v>
-      </c>
-      <c r="J16" t="s">
-        <v>8</v>
+        <v>1</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="B17" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C17" t="s">
-        <v>1</v>
-      </c>
-      <c r="D17" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E17" t="s">
         <v>3</v>
@@ -1623,22 +1735,22 @@
       <c r="F17" t="s">
         <v>4</v>
       </c>
-      <c r="H17" t="s">
-        <v>6</v>
-      </c>
       <c r="I17" t="s">
-        <v>7</v>
-      </c>
-      <c r="J17" t="s">
-        <v>8</v>
+        <v>1</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D18" t="s">
-        <v>2</v>
+        <v>35</v>
+      </c>
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" t="s">
+        <v>10</v>
       </c>
       <c r="E18" t="s">
         <v>3</v>
@@ -1646,25 +1758,22 @@
       <c r="F18" t="s">
         <v>4</v>
       </c>
-      <c r="H18" t="s">
-        <v>6</v>
-      </c>
-      <c r="I18" t="s">
-        <v>7</v>
-      </c>
-      <c r="J18" t="s">
-        <v>8</v>
+      <c r="G18" t="s">
+        <v>5</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="B19" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C19" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D19" t="s">
         <v>2</v>
@@ -1675,25 +1784,25 @@
       <c r="F19" t="s">
         <v>4</v>
       </c>
-      <c r="H19" t="s">
-        <v>6</v>
+      <c r="G19" t="s">
+        <v>5</v>
       </c>
       <c r="I19" t="s">
-        <v>7</v>
-      </c>
-      <c r="J19" t="s">
-        <v>8</v>
+        <v>1</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="B20" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C20" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D20" t="s">
         <v>2</v>
@@ -1704,25 +1813,28 @@
       <c r="F20" t="s">
         <v>4</v>
       </c>
+      <c r="G20" t="s">
+        <v>5</v>
+      </c>
       <c r="H20" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I20" t="s">
-        <v>7</v>
-      </c>
-      <c r="J20" t="s">
-        <v>8</v>
+        <v>1</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="B21" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C21" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D21" t="s">
         <v>2</v>
@@ -1733,25 +1845,28 @@
       <c r="F21" t="s">
         <v>4</v>
       </c>
+      <c r="G21" t="s">
+        <v>5</v>
+      </c>
       <c r="H21" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I21" t="s">
-        <v>7</v>
-      </c>
-      <c r="J21" t="s">
-        <v>8</v>
+        <v>1</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="B22" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C22" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D22" t="s">
         <v>2</v>
@@ -1762,59 +1877,86 @@
       <c r="F22" t="s">
         <v>4</v>
       </c>
+      <c r="G22" t="s">
+        <v>5</v>
+      </c>
+      <c r="H22" t="s">
+        <v>0</v>
+      </c>
       <c r="I22" t="s">
+        <v>1</v>
+      </c>
+      <c r="J22" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="B23" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C23" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D23" t="s">
         <v>2</v>
       </c>
+      <c r="E23" t="s">
+        <v>3</v>
+      </c>
       <c r="F23" t="s">
         <v>4</v>
       </c>
+      <c r="G23" t="s">
+        <v>5</v>
+      </c>
+      <c r="H23" t="s">
+        <v>0</v>
+      </c>
       <c r="I23" t="s">
+        <v>1</v>
+      </c>
+      <c r="J23" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="B24" t="s">
-        <v>0</v>
-      </c>
-      <c r="C24" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D24" t="s">
         <v>2</v>
       </c>
+      <c r="E24" t="s">
+        <v>3</v>
+      </c>
       <c r="F24" t="s">
         <v>4</v>
       </c>
+      <c r="G24" t="s">
+        <v>5</v>
+      </c>
+      <c r="H24" t="s">
+        <v>0</v>
+      </c>
       <c r="I24" t="s">
+        <v>1</v>
+      </c>
+      <c r="J24" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="B25" t="s">
-        <v>0</v>
-      </c>
-      <c r="C25" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D25" t="s">
         <v>2</v>
@@ -1825,10 +1967,28 @@
       <c r="F25" t="s">
         <v>4</v>
       </c>
+      <c r="G25" t="s">
+        <v>5</v>
+      </c>
+      <c r="H25" t="s">
+        <v>0</v>
+      </c>
+      <c r="I25" t="s">
+        <v>1</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>35</v>
+        <v>43</v>
+      </c>
+      <c r="B26" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" t="s">
+        <v>10</v>
       </c>
       <c r="D26" t="s">
         <v>2</v>
@@ -1839,13 +1999,28 @@
       <c r="F26" t="s">
         <v>4</v>
       </c>
+      <c r="G26" t="s">
+        <v>5</v>
+      </c>
+      <c r="H26" t="s">
+        <v>0</v>
+      </c>
+      <c r="I26" t="s">
+        <v>1</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="B27" t="s">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="C27" t="s">
+        <v>10</v>
       </c>
       <c r="D27" t="s">
         <v>2</v>
@@ -1856,16 +2031,28 @@
       <c r="F27" t="s">
         <v>4</v>
       </c>
+      <c r="G27" t="s">
+        <v>5</v>
+      </c>
+      <c r="H27" t="s">
+        <v>0</v>
+      </c>
+      <c r="I27" t="s">
+        <v>1</v>
+      </c>
+      <c r="J27" s="3" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="B28" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C28" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D28" t="s">
         <v>2</v>
@@ -1876,16 +2063,28 @@
       <c r="F28" t="s">
         <v>4</v>
       </c>
+      <c r="G28" t="s">
+        <v>5</v>
+      </c>
+      <c r="H28" t="s">
+        <v>0</v>
+      </c>
+      <c r="I28" t="s">
+        <v>1</v>
+      </c>
+      <c r="J28" s="3" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="B29" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C29" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D29" t="s">
         <v>2</v>
@@ -1896,6 +2095,24 @@
       <c r="F29" t="s">
         <v>4</v>
       </c>
+      <c r="G29" t="s">
+        <v>5</v>
+      </c>
+      <c r="H29" t="s">
+        <v>0</v>
+      </c>
+      <c r="I29" t="s">
+        <v>1</v>
+      </c>
+      <c r="J29" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30" s="1"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>